<commit_message>
added number of records updated and failed + switched to reason codes
</commit_message>
<xml_diff>
--- a/rfrupload/rfrapp/input/input.xlsx
+++ b/rfrupload/rfrapp/input/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="80" windowWidth="19140" windowHeight="7340"/>
+    <workbookView xWindow="320" yWindow="360" windowWidth="18820" windowHeight="7060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Category</t>
   </si>
@@ -72,10 +72,16 @@
     <t>Corrected Reasons by Planners</t>
   </si>
   <si>
-    <t>Discontinued/ Obsolete</t>
-  </si>
-  <si>
-    <t>Sales Related</t>
+    <t>O2</t>
+  </si>
+  <si>
+    <t>RJ</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>SO</t>
   </si>
 </sst>
 </file>
@@ -414,15 +420,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="9" max="9" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
@@ -501,6 +507,28 @@
       </c>
       <c r="R3" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="C4">
+        <v>1601002</v>
+      </c>
+      <c r="N4">
+        <v>102343878</v>
+      </c>
+      <c r="R4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="C5">
+        <v>1600544</v>
+      </c>
+      <c r="N5">
+        <v>102343878</v>
+      </c>
+      <c r="R5" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>